<commit_message>
update core 2_3 trimester variables
</commit_message>
<xml_diff>
--- a/dictionaries/core/2_3/2_3_trimester_rep.xlsx
+++ b/dictionaries/core/2_3/2_3_trimester_rep.xlsx
@@ -620,34 +620,34 @@
     <t xml:space="preserve">distance to meteorological station</t>
   </si>
   <si>
-    <t xml:space="preserve">SAI_score_t1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAI score first trimester</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCL_total_score_t1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCL score first trimester</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCL_anx_score_t1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCL anxiety score first trimester</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCL_dep_score_t1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCL depression score first trimester</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GA_anx_t1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestational age in days at first trimester anxiety measure</t>
+    <t xml:space="preserve">SAI_score_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAI score X trimester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCL_total_score_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCL score X trimester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCL_anx_score_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCL anxiety score X trimester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCL_dep_score_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCL depression score X trimester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GA_anx_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestational age in days at X trimester anxiety measure</t>
   </si>
   <si>
     <t xml:space="preserve">variable</t>
@@ -921,13 +921,13 @@
   </sheetPr>
   <dimension ref="A1:D317"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A93" activeCellId="0" sqref="A93"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D93" activeCellId="0" sqref="D93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.42"/>
@@ -3604,7 +3604,7 @@
       <selection pane="bottomLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.42"/>

</xml_diff>